<commit_message>
240104 - poi library 설치 완료 / 달력 날짜 출력 완료
날짜 출력와 스타일 복사는 완료했지만 빈 행에 스타일 적용을 아직 못 함
이중반복문을 이용해 해결해야 될 거 같다고 생각하고 있고 패턴 분석이 원활하지 않음 내일까지 완성하는 게 목표
</commit_message>
<xml_diff>
--- a/달력폼.xlsx
+++ b/달력폼.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\worktraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2BF3CE-170E-4BE9-9217-AAD19B1B6232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D0A448-7AA2-4595-9E8E-944C2A7ADF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1644" yWindow="2460" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -445,33 +444,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="2"/>
+      <c r="C2" s="3"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="C3" s="3"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B5" s="5"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>